<commit_message>
Added recovery years as a explanatory variable, hoping that accounting for this variation we can tease out better temperature characteristics
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\chapter1_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A15895-E273-4414-86A8-A49B13773C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115DA56A-8F1B-4C85-B196-5A6EBDFF99D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5BF1B947-5B26-479F-8156-42CBDD83DA17}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5548" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5549" uniqueCount="1098">
   <si>
     <t>Name of Hibernaculum</t>
   </si>
@@ -4106,9 +4106,9 @@
   <dimension ref="A1:AL599"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A591" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A486" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="A332" sqref="A332"/>
+      <selection pane="bottomLeft" activeCell="A450" sqref="A450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28703,7 +28703,9 @@
       </c>
     </row>
     <row r="449" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A449" s="35"/>
+      <c r="A449" s="35" t="s">
+        <v>826</v>
+      </c>
       <c r="B449" s="35"/>
       <c r="C449" s="35"/>
       <c r="D449" s="35"/>

</xml_diff>